<commit_message>
Cookie checker relative path
</commit_message>
<xml_diff>
--- a/CookieChecker/IE-CookiesDef.xlsx
+++ b/CookieChecker/IE-CookiesDef.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
   <si>
     <t>Domain</t>
   </si>
@@ -461,17 +461,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -490,58 +490,79 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -549,88 +570,142 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
       <c r="B15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -641,39 +716,75 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
       <c r="B22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
       <c r="B23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -681,89 +792,191 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
       <c r="B25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
       <c r="B26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
       <c r="B27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
       <c r="B28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
       <c r="B30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
       <c r="B31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
       <c r="B32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
       <c r="B33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>